<commit_message>
edit standard page limit and add one mode && edit downloadScoreTemplate pos
</commit_message>
<xml_diff>
--- a/app/static/uploadTemplate/学校信息导入模板.xlsx
+++ b/app/static/uploadTemplate/学校信息导入模板.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA6006D-B49E-4756-8F84-5BF8A6FAD3EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="4875" yWindow="2490" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="22995" windowHeight="9900"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -28,19 +22,25 @@
     <t>学校代码</t>
   </si>
   <si>
-    <t>学校类比</t>
+    <t>学校类别</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -48,26 +48,356 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -75,27 +405,313 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
+    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
+    <cellStyle name="输入" xfId="4" builtinId="20"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
+    <cellStyle name="货币" xfId="7" builtinId="4"/>
+    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
+    <cellStyle name="百分比" xfId="9" builtinId="5"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
+    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
+    <cellStyle name="计算" xfId="15" builtinId="22"/>
+    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
+    <cellStyle name="适中" xfId="17" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
+    <cellStyle name="好" xfId="19" builtinId="26"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="差" xfId="22" builtinId="27"/>
+    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
+    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
+    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
+    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
+    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
+    <cellStyle name="标题" xfId="33" builtinId="15"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
+    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="注释" xfId="37" builtinId="10"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
+    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8"/>
+    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
+    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
+    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -144,7 +760,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -177,26 +793,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -229,23 +828,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -253,7 +835,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -274,9 +856,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="16200000" scaled="true"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -297,7 +879,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="16200000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -367,7 +949,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -393,7 +975,7 @@
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -416,22 +998,24 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="2"/>
   <cols>
-    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,16 +1027,13 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{6B890BA0-4D4C-4B5B-AD77-7F70004F2327}">
-      <formula1>"本科,高职高专"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="提示" prompt="请填入本科或者高职高专" sqref="C1" xr:uid="{2D8C6718-7F0E-4594-BEAB-8629ECAAD219}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="提示" prompt="请填入本科或者高职高专" sqref="C$1:C$1048576">
       <formula1>"本科,高职高专"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>